<commit_message>
adding Fick's diffusion, editing gitignore
</commit_message>
<xml_diff>
--- a/macrophage_model.xlsx
+++ b/macrophage_model.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Library/CloudStorage/iCloud Drive/Documents/Summer/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F39907-02ED-0B45-A215-0BAD2661DBDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA131AA-91AD-E24B-9D2B-16A1059D0A8F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="540" windowWidth="25440" windowHeight="16780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8100" yWindow="540" windowWidth="25440" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
     <sheet name="reactions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="140">
   <si>
     <t>Species information</t>
   </si>
@@ -442,9 +441,6 @@
   </si>
   <si>
     <t>nuclear factor kappa</t>
-  </si>
-  <si>
-    <t>model id</t>
   </si>
 </sst>
 </file>
@@ -562,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -613,12 +609,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1002,209 +992,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DL37"/>
+  <dimension ref="A1:DK37"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" s="7" customFormat="1">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:115" s="7" customFormat="1">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-    </row>
-    <row r="2" spans="1:116" s="3" customFormat="1">
-      <c r="A2" s="26" t="s">
-        <v>140</v>
+    </row>
+    <row r="2" spans="1:115" s="3" customFormat="1">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:115" ht="18" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="20">
         <v>1</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:116" ht="18" customHeight="1">
-      <c r="A3" s="25">
-        <v>0</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="E3" s="20">
         <v>1</v>
       </c>
       <c r="F3" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:115">
+      <c r="A4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20">
         <v>1</v>
       </c>
-      <c r="G3" s="20">
+      <c r="F4" s="20">
         <v>0.1</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="G4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:115">
+      <c r="A5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="1:115">
+      <c r="A6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-    </row>
-    <row r="4" spans="1:116">
-      <c r="A4" s="25">
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="1:115" s="2" customFormat="1">
+      <c r="A7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
         <v>1</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="20">
-        <v>0</v>
-      </c>
-      <c r="F4" s="20">
-        <v>1</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="F7" s="20">
         <v>0.1</v>
       </c>
-      <c r="H4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:116">
-      <c r="A5" s="25">
-        <v>2</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="20">
-        <v>0</v>
-      </c>
-      <c r="F5" s="20">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-    </row>
-    <row r="6" spans="1:116">
-      <c r="A6" s="25">
-        <v>3</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="20">
-        <v>0</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="H6" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:116" s="2" customFormat="1">
-      <c r="A7" s="25">
-        <v>4</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="20">
-        <v>0</v>
-      </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="H7" s="20"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
@@ -1310,37 +1283,34 @@
       <c r="DI7"/>
       <c r="DJ7"/>
       <c r="DK7"/>
-      <c r="DL7"/>
-    </row>
-    <row r="8" spans="1:116" s="2" customFormat="1">
-      <c r="A8" s="25">
-        <v>5</v>
+    </row>
+    <row r="8" spans="1:115" s="2" customFormat="1">
+      <c r="A8" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="20" t="s">
         <v>105</v>
       </c>
+      <c r="D8" s="20">
+        <v>0</v>
+      </c>
       <c r="E8" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="20">
         <v>1</v>
       </c>
-      <c r="G8" s="20">
-        <v>1</v>
+      <c r="G8" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
@@ -1446,125 +1416,113 @@
       <c r="DI8"/>
       <c r="DJ8"/>
       <c r="DK8"/>
-      <c r="DL8"/>
-    </row>
-    <row r="9" spans="1:116">
-      <c r="A9" s="25">
-        <v>6</v>
+    </row>
+    <row r="9" spans="1:115">
+      <c r="A9" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:115">
+      <c r="A10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="20">
+      <c r="B10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="20">
         <v>0</v>
       </c>
-      <c r="F9" s="20">
+      <c r="E10" s="20">
         <v>1</v>
       </c>
-      <c r="G9" s="20">
+      <c r="F10" s="20">
         <v>0.1</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="G10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:116">
-      <c r="A10" s="25">
-        <v>7</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="H10" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="1:115">
+      <c r="A11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="20">
+      <c r="B11" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="20">
         <v>0</v>
       </c>
-      <c r="F10" s="20">
+      <c r="E11" s="20">
         <v>1</v>
       </c>
-      <c r="G10" s="20">
+      <c r="F11" s="20">
         <v>0.1</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="G11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:116">
-      <c r="A11" s="25">
-        <v>8</v>
-      </c>
-      <c r="B11" s="20" t="s">
+      <c r="H11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:115" s="2" customFormat="1">
+      <c r="A12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="20" t="s">
+      <c r="B12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="20">
+      <c r="D12" s="20">
         <v>0</v>
       </c>
-      <c r="F11" s="20">
+      <c r="E12" s="20">
         <v>1</v>
       </c>
-      <c r="G11" s="20">
+      <c r="F12" s="20">
         <v>0.1</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="G12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:116" s="2" customFormat="1">
-      <c r="A12" s="25">
-        <v>9</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="20">
-        <v>0</v>
-      </c>
-      <c r="F12" s="20">
-        <v>1</v>
-      </c>
-      <c r="G12" s="20">
-        <v>0.1</v>
-      </c>
       <c r="H12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
@@ -1670,35 +1628,32 @@
       <c r="DI12"/>
       <c r="DJ12"/>
       <c r="DK12"/>
-      <c r="DL12"/>
-    </row>
-    <row r="13" spans="1:116" s="2" customFormat="1">
-      <c r="A13" s="25">
-        <v>10</v>
+    </row>
+    <row r="13" spans="1:115" s="2" customFormat="1">
+      <c r="A13" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="20" t="s">
         <v>23</v>
       </c>
+      <c r="D13" s="20">
+        <v>0</v>
+      </c>
       <c r="E13" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="20">
-        <v>1</v>
-      </c>
-      <c r="G13" s="20">
         <v>0.1</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="G13" s="20" t="s">
         <v>11</v>
       </c>
+      <c r="H13" s="20"/>
       <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
+      <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -1804,65 +1759,59 @@
       <c r="DI13"/>
       <c r="DJ13"/>
       <c r="DK13"/>
-      <c r="DL13"/>
-    </row>
-    <row r="14" spans="1:116">
-      <c r="A14" s="25">
+    </row>
+    <row r="14" spans="1:115">
+      <c r="A14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" s="20">
+      <c r="H14" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:115" s="2" customFormat="1">
+      <c r="A15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="20">
         <v>0</v>
       </c>
-      <c r="F14" s="20">
+      <c r="E15" s="20">
         <v>1</v>
-      </c>
-      <c r="G14" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:116" s="2" customFormat="1">
-      <c r="A15" s="25">
-        <v>12</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="20">
-        <v>0</v>
       </c>
       <c r="F15" s="20">
         <v>1</v>
       </c>
-      <c r="G15" s="20">
-        <v>1</v>
-      </c>
-      <c r="H15" s="20" t="s">
+      <c r="G15" s="20" t="s">
         <v>11</v>
       </c>
+      <c r="H15" s="20"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
+      <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -1968,265 +1917,238 @@
       <c r="DI15"/>
       <c r="DJ15"/>
       <c r="DK15"/>
-      <c r="DL15"/>
-    </row>
-    <row r="16" spans="1:116">
-      <c r="A16" s="25">
-        <v>13</v>
+    </row>
+    <row r="16" spans="1:115">
+      <c r="A16" s="20" t="s">
+        <v>16</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="20" t="s">
         <v>19</v>
       </c>
+      <c r="D16" s="20">
+        <v>0</v>
+      </c>
       <c r="E16" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="20">
         <v>1</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0</v>
+      </c>
+      <c r="E17" s="20">
         <v>1</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="25">
-        <v>14</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="20">
-        <v>0</v>
       </c>
       <c r="F17" s="20">
         <v>1</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
+      <c r="E18" s="20">
         <v>1</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="F18" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="25">
-        <v>15</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="20">
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="20">
         <v>0</v>
       </c>
-      <c r="F18" s="20">
+      <c r="E19" s="20">
         <v>1</v>
-      </c>
-      <c r="G18" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="25">
-        <v>16</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="20">
-        <v>0</v>
       </c>
       <c r="F19" s="20">
         <v>1</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20">
         <v>1</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="25">
-        <v>17</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="20">
-        <v>0</v>
       </c>
       <c r="F20" s="20">
         <v>1</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0</v>
+      </c>
+      <c r="E21" s="20">
         <v>1</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="25">
-        <v>18</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="20">
-        <v>0</v>
       </c>
       <c r="F21" s="20">
         <v>1</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="20">
+        <v>0</v>
+      </c>
+      <c r="E22" s="20">
         <v>1</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="25">
-        <v>19</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="20">
-        <v>0</v>
       </c>
       <c r="F22" s="20">
         <v>1</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="24"/>
+      <c r="D23" s="20">
+        <v>0</v>
+      </c>
+      <c r="E23" s="20">
         <v>1</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="25">
-        <v>20</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="20">
-        <v>0</v>
       </c>
       <c r="F23" s="20">
         <v>1</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="20">
         <v>1</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="25">
-        <v>21</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="20">
-        <v>0</v>
       </c>
       <c r="F24" s="20">
         <v>1</v>
       </c>
-      <c r="G24" s="20">
-        <v>1</v>
-      </c>
-      <c r="H24" s="20" t="s">
+      <c r="G24" s="20" t="s">
         <v>121</v>
       </c>
+      <c r="H24" s="24"/>
       <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
@@ -2235,9 +2157,9 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
@@ -2246,9 +2168,9 @@
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -2257,9 +2179,9 @@
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -2268,9 +2190,9 @@
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -2279,9 +2201,9 @@
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -2290,9 +2212,9 @@
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -2301,9 +2223,9 @@
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
@@ -2312,9 +2234,9 @@
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
-      <c r="J32"/>
-    </row>
-    <row r="33" spans="2:10">
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
@@ -2323,9 +2245,9 @@
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
-      <c r="J33"/>
-    </row>
-    <row r="34" spans="2:10">
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
@@ -2334,9 +2256,9 @@
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
-      <c r="J34"/>
-    </row>
-    <row r="35" spans="2:10">
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
@@ -2345,9 +2267,9 @@
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>
-      <c r="J35"/>
-    </row>
-    <row r="36" spans="2:10">
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
@@ -2356,9 +2278,9 @@
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
-      <c r="J36"/>
-    </row>
-    <row r="37" spans="2:10">
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
@@ -2367,7 +2289,6 @@
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
-      <c r="J37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2380,8 +2301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AY125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add new sensitivity analysis data
</commit_message>
<xml_diff>
--- a/macrophage_model.xlsx
+++ b/macrophage_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Library/CloudStorage/iCloud Drive/Documents/Summer/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976E517E-62E9-BE47-9D5C-102D065100AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0E4A6D-9586-B245-B379-D59C082D0A99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16760" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19660" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:DK43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>